<commit_message>
Commit current WIP excel manipulation tools.
</commit_message>
<xml_diff>
--- a/py/tables/TestTable.xlsx
+++ b/py/tables/TestTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan.fleck\Documents\Projects\py\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3240CA-5B5F-4A05-AE38-CA81B39821E0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7976A9E9-5394-42BA-9700-69D3E1BC589F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24510" activeTab="2" xr2:uid="{36F798D4-741A-4AF5-9482-CC9834C01A80}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t>Test Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Add another row to see data shape</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -596,13 +602,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B104AC73-76FD-4658-A95E-58B56B41F4A6}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -681,6 +690,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>